<commit_message>
First modifications of the code
</commit_message>
<xml_diff>
--- a/Met Office named storms.xlsx
+++ b/Met Office named storms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://defra.sharepoint.com/teams/Team3580/Team Documents/Incident Management/Past incidents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPHILLIPS03\Documents\repos\historicfloodlevels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23B834A0-A970-4F9A-8C4B-B2662B73046A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E4AC39-EEB4-49BC-9061-D4A34C417175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7335D6D-99A8-4784-9B00-28C6F274A856}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24060" windowHeight="9630" xr2:uid="{F7335D6D-99A8-4784-9B00-28C6F274A856}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -44,16 +44,7 @@
     <t>Date named</t>
   </si>
   <si>
-    <t>Start date of impacts on UK and/or Ireland and/or Netherlands</t>
-  </si>
-  <si>
-    <t>End date of impacts on UK and/or Ireland and/or Netherlands</t>
-  </si>
-  <si>
     <t>Abigail</t>
-  </si>
-  <si>
-    <t>Data taken from Met Office</t>
   </si>
   <si>
     <t>Barney</t>
@@ -290,7 +281,10 @@
     <t>Isha &amp; Jocelyn</t>
   </si>
   <si>
-    <t>* impact dates specified within EA recovery cell</t>
+    <t>startdate</t>
+  </si>
+  <si>
+    <t>enddate</t>
   </si>
 </sst>
 </file>
@@ -300,7 +294,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -626,9 +620,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -657,6 +648,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -997,19 +994,20 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="6" width="9.140625" style="23"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="50.25" customHeight="1" thickBot="1">
+    <row r="1" spans="1:6" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1017,37 +1015,35 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="B2" s="13">
+        <v>42318</v>
+      </c>
+      <c r="C2" s="14">
+        <v>42320</v>
+      </c>
+      <c r="D2" s="15">
+        <v>42321</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="14">
-        <v>42318</v>
-      </c>
-      <c r="C2" s="15">
-        <v>42320</v>
-      </c>
-      <c r="D2" s="16">
-        <v>42321</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="17">
+      <c r="B3" s="16">
         <v>42324</v>
       </c>
       <c r="C3" s="4">
@@ -1056,14 +1052,14 @@
       <c r="D3" s="5">
         <v>42326</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="17">
+        <v>4</v>
+      </c>
+      <c r="B4" s="16">
         <v>42336</v>
       </c>
       <c r="C4" s="4">
@@ -1072,14 +1068,14 @@
       <c r="D4" s="5">
         <v>42337</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="17">
+        <v>5</v>
+      </c>
+      <c r="B5" s="16">
         <v>42342</v>
       </c>
       <c r="C5" s="4">
@@ -1088,14 +1084,14 @@
       <c r="D5" s="5">
         <v>42344</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="17">
+        <v>6</v>
+      </c>
+      <c r="B6" s="16">
         <v>42360</v>
       </c>
       <c r="C6" s="4">
@@ -1104,14 +1100,14 @@
       <c r="D6" s="5">
         <v>42362</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="17">
+        <v>7</v>
+      </c>
+      <c r="B7" s="16">
         <v>42366</v>
       </c>
       <c r="C7" s="4">
@@ -1120,14 +1116,14 @@
       <c r="D7" s="5">
         <v>42368</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="17">
+        <v>8</v>
+      </c>
+      <c r="B8" s="16">
         <v>42397</v>
       </c>
       <c r="C8" s="4">
@@ -1136,14 +1132,14 @@
       <c r="D8" s="5">
         <v>42398</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="17">
+        <v>9</v>
+      </c>
+      <c r="B9" s="16">
         <v>42399</v>
       </c>
       <c r="C9" s="4">
@@ -1152,14 +1148,14 @@
       <c r="D9" s="5">
         <v>42402</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="17">
+        <v>10</v>
+      </c>
+      <c r="B10" s="16">
         <v>42407</v>
       </c>
       <c r="C10" s="4">
@@ -1168,14 +1164,14 @@
       <c r="D10" s="5">
         <v>42408</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="17">
+        <v>11</v>
+      </c>
+      <c r="B11" s="16">
         <v>42430</v>
       </c>
       <c r="C11" s="4">
@@ -1184,14 +1180,14 @@
       <c r="D11" s="5">
         <v>42431</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="17">
+        <v>12</v>
+      </c>
+      <c r="B12" s="16">
         <v>42454</v>
       </c>
       <c r="C12" s="4">
@@ -1200,14 +1196,14 @@
       <c r="D12" s="5">
         <v>42457</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="17">
+        <v>13</v>
+      </c>
+      <c r="B13" s="16">
         <v>42693</v>
       </c>
       <c r="C13" s="4">
@@ -1216,14 +1212,14 @@
       <c r="D13" s="5">
         <v>42694</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="17">
+        <v>14</v>
+      </c>
+      <c r="B14" s="16">
         <v>42724</v>
       </c>
       <c r="C14" s="4">
@@ -1232,14 +1228,14 @@
       <c r="D14" s="5">
         <v>42728</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="17">
+        <v>15</v>
+      </c>
+      <c r="B15" s="16">
         <v>42727</v>
       </c>
       <c r="C15" s="4">
@@ -1248,14 +1244,14 @@
       <c r="D15" s="5">
         <v>42730</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="17">
+        <v>16</v>
+      </c>
+      <c r="B16" s="16">
         <v>42787</v>
       </c>
       <c r="C16" s="4">
@@ -1264,14 +1260,14 @@
       <c r="D16" s="5">
         <v>42789</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="16">
         <v>42791</v>
       </c>
       <c r="C17" s="4">
@@ -1281,12 +1277,12 @@
         <v>42792</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C18" s="4">
         <v>42990</v>
@@ -1295,12 +1291,12 @@
         <v>42991</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C19" s="4">
         <v>43024</v>
@@ -1309,9 +1305,9 @@
         <v>43025</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B20" s="10">
         <v>43027</v>
@@ -1323,9 +1319,9 @@
         <v>43029</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B21" s="10">
         <v>43074</v>
@@ -1337,9 +1333,9 @@
         <v>43076</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B22" s="10">
         <v>43098</v>
@@ -1351,9 +1347,9 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B23" s="10">
         <v>43101</v>
@@ -1365,9 +1361,9 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B24" s="10">
         <v>43116</v>
@@ -1379,12 +1375,12 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="C25" s="4">
         <v>43118</v>
@@ -1393,9 +1389,9 @@
         <v>43118</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B26" s="10">
         <v>43123</v>
@@ -1407,9 +1403,9 @@
         <v>43124</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B27" s="10">
         <v>43264</v>
@@ -1421,11 +1417,11 @@
         <v>43265</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="17">
+        <v>31</v>
+      </c>
+      <c r="B28" s="16">
         <v>43361</v>
       </c>
       <c r="C28" s="4">
@@ -1435,11 +1431,11 @@
         <v>43362</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="17">
+        <v>32</v>
+      </c>
+      <c r="B29" s="16">
         <v>43363</v>
       </c>
       <c r="C29" s="4">
@@ -1449,11 +1445,11 @@
         <v>43364</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="17">
+        <v>33</v>
+      </c>
+      <c r="B30" s="16">
         <v>43383</v>
       </c>
       <c r="C30" s="4">
@@ -1463,11 +1459,11 @@
         <v>43386</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="17">
+        <v>34</v>
+      </c>
+      <c r="B31" s="16">
         <v>43448</v>
       </c>
       <c r="C31" s="4">
@@ -1477,11 +1473,11 @@
         <v>43450</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="17">
+        <v>35</v>
+      </c>
+      <c r="B32" s="16">
         <v>43503</v>
       </c>
       <c r="C32" s="4">
@@ -1491,11 +1487,11 @@
         <v>43505</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="17">
+        <v>36</v>
+      </c>
+      <c r="B33" s="16">
         <v>43525</v>
       </c>
       <c r="C33" s="4">
@@ -1505,11 +1501,11 @@
         <v>43528</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="17">
+        <v>37</v>
+      </c>
+      <c r="B34" s="16">
         <v>43535</v>
       </c>
       <c r="C34" s="4">
@@ -1519,11 +1515,11 @@
         <v>43537</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B35" s="17">
+        <v>38</v>
+      </c>
+      <c r="B35" s="16">
         <v>43581</v>
       </c>
       <c r="C35" s="4">
@@ -1533,11 +1529,11 @@
         <v>43582</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="17">
+        <v>39</v>
+      </c>
+      <c r="B36" s="16">
         <v>43805</v>
       </c>
       <c r="C36" s="4">
@@ -1547,11 +1543,11 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="17">
+        <v>40</v>
+      </c>
+      <c r="B37" s="16">
         <v>43841</v>
       </c>
       <c r="C37" s="4">
@@ -1561,11 +1557,11 @@
         <v>43844</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="17">
+        <v>41</v>
+      </c>
+      <c r="B38" s="16">
         <v>43866</v>
       </c>
       <c r="C38" s="4">
@@ -1575,11 +1571,11 @@
         <v>43870</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="17">
+        <v>42</v>
+      </c>
+      <c r="B39" s="16">
         <v>43872</v>
       </c>
       <c r="C39" s="4">
@@ -1589,12 +1585,12 @@
         <v>43876</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>44</v>
       </c>
       <c r="C40" s="4">
         <v>43889</v>
@@ -1603,11 +1599,11 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B41" s="17">
+        <v>45</v>
+      </c>
+      <c r="B41" s="16">
         <v>44061</v>
       </c>
       <c r="C41" s="4">
@@ -1617,11 +1613,11 @@
         <v>44063</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" s="17">
+        <v>46</v>
+      </c>
+      <c r="B42" s="16">
         <v>44067</v>
       </c>
       <c r="C42" s="4">
@@ -1631,12 +1627,12 @@
         <v>44069</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>48</v>
       </c>
       <c r="C43" s="4">
         <v>44106</v>
@@ -1645,12 +1641,12 @@
         <v>44108</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>52</v>
+        <v>14</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="C44" s="4">
         <v>44125</v>
@@ -1659,11 +1655,11 @@
         <v>44125</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45" s="17">
+        <v>50</v>
+      </c>
+      <c r="B45" s="16">
         <v>44134</v>
       </c>
       <c r="C45" s="4">
@@ -1673,11 +1669,11 @@
         <v>44135</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="17">
+        <v>51</v>
+      </c>
+      <c r="B46" s="16">
         <v>44189</v>
       </c>
       <c r="C46" s="4">
@@ -1687,11 +1683,11 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" s="17">
+        <v>52</v>
+      </c>
+      <c r="B47" s="16">
         <v>44214</v>
       </c>
       <c r="C47" s="4">
@@ -1701,12 +1697,12 @@
         <v>44218</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>54</v>
       </c>
       <c r="C48" s="4">
         <v>44233</v>
@@ -1715,11 +1711,11 @@
         <v>44235</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" s="17">
+        <v>55</v>
+      </c>
+      <c r="B49" s="16">
         <v>44406</v>
       </c>
       <c r="C49" s="4">
@@ -1729,11 +1725,11 @@
         <v>44407</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B50" s="17">
+        <v>56</v>
+      </c>
+      <c r="B50" s="16">
         <v>44525</v>
       </c>
       <c r="C50" s="4">
@@ -1743,11 +1739,11 @@
         <v>44527</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B51" s="17">
+        <v>57</v>
+      </c>
+      <c r="B51" s="16">
         <v>44535</v>
       </c>
       <c r="C51" s="4">
@@ -1757,12 +1753,12 @@
         <v>44538</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>59</v>
       </c>
       <c r="C52" s="4">
         <v>44590</v>
@@ -1771,11 +1767,11 @@
         <v>44590</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="17">
+        <v>60</v>
+      </c>
+      <c r="B53" s="16">
         <v>44590</v>
       </c>
       <c r="C53" s="4">
@@ -1785,11 +1781,11 @@
         <v>44592</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="17">
+        <v>61</v>
+      </c>
+      <c r="B54" s="16">
         <v>44606</v>
       </c>
       <c r="C54" s="4">
@@ -1799,11 +1795,11 @@
         <v>44609</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" s="17">
+        <v>62</v>
+      </c>
+      <c r="B55" s="16">
         <v>44606</v>
       </c>
       <c r="C55" s="4">
@@ -1813,11 +1809,11 @@
         <v>44610</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B56" s="17">
+        <v>63</v>
+      </c>
+      <c r="B56" s="16">
         <v>44612</v>
       </c>
       <c r="C56" s="4">
@@ -1827,12 +1823,12 @@
         <v>44613</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>68</v>
+        <v>64</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>65</v>
       </c>
       <c r="C57" s="4">
         <v>44974</v>
@@ -1841,12 +1837,12 @@
         <v>44974</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="C58" s="4">
         <v>45028</v>
@@ -1855,11 +1851,11 @@
         <v>45028</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B59" s="17">
+        <v>68</v>
+      </c>
+      <c r="B59" s="16">
         <v>45142</v>
       </c>
       <c r="C59" s="4">
@@ -1869,11 +1865,11 @@
         <v>45143</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B60" s="17">
+        <v>69</v>
+      </c>
+      <c r="B60" s="16">
         <v>45156</v>
       </c>
       <c r="C60" s="4">
@@ -1883,11 +1879,11 @@
         <v>45157</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B61" s="17">
+        <v>70</v>
+      </c>
+      <c r="B61" s="16">
         <v>45194</v>
       </c>
       <c r="C61" s="4">
@@ -1897,116 +1893,114 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" s="16">
+        <v>45215</v>
+      </c>
+      <c r="C62" s="17">
+        <v>45217</v>
+      </c>
+      <c r="D62" s="18">
+        <v>45230</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="16">
+        <v>45228</v>
+      </c>
+      <c r="C63" s="17">
+        <v>45231</v>
+      </c>
+      <c r="D63" s="18">
+        <v>45238</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" s="16">
+        <v>45242</v>
+      </c>
+      <c r="C64" s="17">
+        <v>45243</v>
+      </c>
+      <c r="D64" s="18">
+        <v>45243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B62" s="17">
-        <v>45215</v>
-      </c>
-      <c r="C62" s="18">
-        <v>45217</v>
-      </c>
-      <c r="D62" s="19">
-        <v>45230</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="8" t="s">
+      <c r="B65" s="16">
+        <v>45269</v>
+      </c>
+      <c r="C65" s="17">
+        <v>45239</v>
+      </c>
+      <c r="D65" s="18">
+        <v>45247</v>
+      </c>
+      <c r="E65" s="22"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B63" s="17">
-        <v>45228</v>
-      </c>
-      <c r="C63" s="18">
-        <v>45231</v>
-      </c>
-      <c r="D63" s="19">
-        <v>45238</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="8" t="s">
+      <c r="B66" s="16">
+        <v>45286</v>
+      </c>
+      <c r="C66" s="17">
+        <v>45286</v>
+      </c>
+      <c r="D66" s="18">
+        <v>45293</v>
+      </c>
+      <c r="E66" s="22"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B64" s="17">
-        <v>45242</v>
-      </c>
-      <c r="C64" s="18">
-        <v>45243</v>
-      </c>
-      <c r="D64" s="19">
-        <v>45243</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="8" t="s">
+      <c r="B67" s="16">
+        <v>45293</v>
+      </c>
+      <c r="C67" s="17">
+        <v>45293</v>
+      </c>
+      <c r="D67" s="18">
+        <v>45302</v>
+      </c>
+      <c r="E67" s="22"/>
+    </row>
+    <row r="68" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B65" s="17">
-        <v>45269</v>
-      </c>
-      <c r="C65" s="18">
-        <v>45239</v>
-      </c>
-      <c r="D65" s="19">
-        <v>45247</v>
-      </c>
-      <c r="E65" s="3"/>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B66" s="17">
-        <v>45286</v>
-      </c>
-      <c r="C66" s="18">
-        <v>45286</v>
-      </c>
-      <c r="D66" s="19">
-        <v>45293</v>
-      </c>
-      <c r="E66" s="3"/>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B67" s="17">
-        <v>45293</v>
-      </c>
-      <c r="C67" s="18">
-        <v>45293</v>
-      </c>
-      <c r="D67" s="19">
-        <v>45302</v>
-      </c>
-      <c r="E67" s="3"/>
-    </row>
-    <row r="68" spans="1:5" ht="15" thickBot="1">
-      <c r="A68" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B68" s="20">
+      <c r="B68" s="19">
         <v>45310</v>
       </c>
-      <c r="C68" s="21">
+      <c r="C68" s="20">
         <v>45312</v>
       </c>
-      <c r="D68" s="22">
+      <c r="D68" s="21">
         <v>45318</v>
       </c>
-      <c r="E68" s="3"/>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="E68" s="22"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
-      <c r="E70" s="12" t="s">
-        <v>81</v>
-      </c>
+      <c r="E70" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -2015,20 +2009,76 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <cf401361b24e474cb011be6eb76c0e76 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Crown</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">69589897-2828-4761-976e-717fd8e631c9</TermId>
+        </TermInfo>
+      </Terms>
+    </cf401361b24e474cb011be6eb76c0e76>
+    <k85d23755b3a46b5a51451cf336b2e9b xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k85d23755b3a46b5a51451cf336b2e9b>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0dd52018-09d6-445c-a0bf-a7d393e3976c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Topic xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">Team Documents</Topic>
+    <HOMigrated xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">false</HOMigrated>
+    <ddeb1fd0a9ad4436a96525d34737dc44 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Defra Group</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0867f7b3-e76e-40ca-bb1f-5ba341a49230</TermId>
+        </TermInfo>
+      </Terms>
+    </ddeb1fd0a9ad4436a96525d34737dc44>
+    <lae2bfa7b6474897ab4a53f76ea236c7 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">14c80daa-741b-422c-9722-f71693c9ede4</TermId>
+        </TermInfo>
+      </Terms>
+    </lae2bfa7b6474897ab4a53f76ea236c7>
+    <TaxCatchAll xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Value>5</Value>
+      <Value>3</Value>
+      <Value>2</Value>
+      <Value>1</Value>
+      <Value>7</Value>
+    </TaxCatchAll>
+    <fe59e9859d6a491389c5b03567f5dda5 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">EA</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d5f78ddb-b1b6-4328-9877-d7e3ed06fdac</TermId>
+        </TermInfo>
+      </Terms>
+    </fe59e9859d6a491389c5b03567f5dda5>
+    <Team xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">West Midlands Flood Resilience</Team>
+    <n7493b4506bf40e28c373b1e51a33445 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Team</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">ff0485df-0575-416f-802f-e999165821b7</TermId>
+        </TermInfo>
+      </Terms>
+    </n7493b4506bf40e28c373b1e51a33445>
+    <SharedWithUsers xmlns="3706cc3d-17f7-47fa-8868-0fddc39686e3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false" LastSyncTimeStamp="2022-12-23T12:39:58.22Z"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Defra document" ma:contentTypeID="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC0100C9D7CF3DB3A5294495E668133806889C" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d902eb373446766bbf1ab3ec0f91b734">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="662745e8-e224-48e8-a2e3-254862b8c2f5" xmlns:ns3="0dd52018-09d6-445c-a0bf-a7d393e3976c" xmlns:ns4="3706cc3d-17f7-47fa-8868-0fddc39686e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7d15225178a027aa0bf830356bf0872" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="662745e8-e224-48e8-a2e3-254862b8c2f5"/>
@@ -2346,88 +2396,64 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false" LastSyncTimeStamp="2022-12-23T12:39:58.22Z"/>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <cf401361b24e474cb011be6eb76c0e76 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Crown</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">69589897-2828-4761-976e-717fd8e631c9</TermId>
-        </TermInfo>
-      </Terms>
-    </cf401361b24e474cb011be6eb76c0e76>
-    <k85d23755b3a46b5a51451cf336b2e9b xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k85d23755b3a46b5a51451cf336b2e9b>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0dd52018-09d6-445c-a0bf-a7d393e3976c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Topic xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">Team Documents</Topic>
-    <HOMigrated xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">false</HOMigrated>
-    <ddeb1fd0a9ad4436a96525d34737dc44 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Defra Group</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0867f7b3-e76e-40ca-bb1f-5ba341a49230</TermId>
-        </TermInfo>
-      </Terms>
-    </ddeb1fd0a9ad4436a96525d34737dc44>
-    <lae2bfa7b6474897ab4a53f76ea236c7 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">14c80daa-741b-422c-9722-f71693c9ede4</TermId>
-        </TermInfo>
-      </Terms>
-    </lae2bfa7b6474897ab4a53f76ea236c7>
-    <TaxCatchAll xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Value>5</Value>
-      <Value>3</Value>
-      <Value>2</Value>
-      <Value>1</Value>
-      <Value>7</Value>
-    </TaxCatchAll>
-    <fe59e9859d6a491389c5b03567f5dda5 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">EA</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d5f78ddb-b1b6-4328-9877-d7e3ed06fdac</TermId>
-        </TermInfo>
-      </Terms>
-    </fe59e9859d6a491389c5b03567f5dda5>
-    <Team xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">West Midlands Flood Resilience</Team>
-    <n7493b4506bf40e28c373b1e51a33445 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Team</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">ff0485df-0575-416f-802f-e999165821b7</TermId>
-        </TermInfo>
-      </Terms>
-    </n7493b4506bf40e28c373b1e51a33445>
-    <SharedWithUsers xmlns="3706cc3d-17f7-47fa-8868-0fddc39686e3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7CB7080-93A0-4465-A6CA-3DE4F8BEE390}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABFDC2C6-1282-4AD8-85C0-3BFC2D82127B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="662745e8-e224-48e8-a2e3-254862b8c2f5"/>
+    <ds:schemaRef ds:uri="0dd52018-09d6-445c-a0bf-a7d393e3976c"/>
+    <ds:schemaRef ds:uri="3706cc3d-17f7-47fa-8868-0fddc39686e3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F171807-FEE5-4AEA-A638-7AEBE7A4AFFE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65740454-FCBB-4306-863D-880BA6829E5F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="662745e8-e224-48e8-a2e3-254862b8c2f5"/>
+    <ds:schemaRef ds:uri="0dd52018-09d6-445c-a0bf-a7d393e3976c"/>
+    <ds:schemaRef ds:uri="3706cc3d-17f7-47fa-8868-0fddc39686e3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65740454-FCBB-4306-863D-880BA6829E5F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F171807-FEE5-4AEA-A638-7AEBE7A4AFFE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABFDC2C6-1282-4AD8-85C0-3BFC2D82127B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7CB7080-93A0-4465-A6CA-3DE4F8BEE390}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add storm names to peaks
</commit_message>
<xml_diff>
--- a/Met Office named storms.xlsx
+++ b/Met Office named storms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPHILLIPS03\Documents\repos\historicfloodlevels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E4AC39-EEB4-49BC-9061-D4A34C417175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91922EF6-9089-4679-A2A6-0216EF3FD3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24060" windowHeight="9630" xr2:uid="{F7335D6D-99A8-4784-9B00-28C6F274A856}"/>
+    <workbookView xWindow="690" yWindow="495" windowWidth="11640" windowHeight="7950" xr2:uid="{F7335D6D-99A8-4784-9B00-28C6F274A856}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -648,12 +648,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -993,8 +987,8 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1003,8 +997,7 @@
     <col min="2" max="2" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="23"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1020,8 +1013,8 @@
       <c r="D1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -1036,8 +1029,8 @@
       <c r="D2" s="15">
         <v>42321</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -1052,8 +1045,8 @@
       <c r="D3" s="5">
         <v>42326</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1068,8 +1061,8 @@
       <c r="D4" s="5">
         <v>42337</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1084,8 +1077,8 @@
       <c r="D5" s="5">
         <v>42344</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -1100,8 +1093,8 @@
       <c r="D6" s="5">
         <v>42362</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
@@ -1116,8 +1109,8 @@
       <c r="D7" s="5">
         <v>42368</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
@@ -1132,8 +1125,8 @@
       <c r="D8" s="5">
         <v>42398</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
@@ -1148,8 +1141,8 @@
       <c r="D9" s="5">
         <v>42402</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -1164,8 +1157,8 @@
       <c r="D10" s="5">
         <v>42408</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -1180,8 +1173,8 @@
       <c r="D11" s="5">
         <v>42431</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -1196,8 +1189,8 @@
       <c r="D12" s="5">
         <v>42457</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -1212,8 +1205,8 @@
       <c r="D13" s="5">
         <v>42694</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -1228,8 +1221,8 @@
       <c r="D14" s="5">
         <v>42728</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -1244,8 +1237,8 @@
       <c r="D15" s="5">
         <v>42730</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -1260,8 +1253,8 @@
       <c r="D16" s="5">
         <v>42789</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -1943,12 +1936,12 @@
         <v>45269</v>
       </c>
       <c r="C65" s="17">
-        <v>45239</v>
+        <v>45269</v>
       </c>
       <c r="D65" s="18">
-        <v>45247</v>
-      </c>
-      <c r="E65" s="22"/>
+        <v>45277</v>
+      </c>
+      <c r="E65" s="3"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
@@ -1963,7 +1956,7 @@
       <c r="D66" s="18">
         <v>45293</v>
       </c>
-      <c r="E66" s="22"/>
+      <c r="E66" s="3"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
@@ -1978,7 +1971,7 @@
       <c r="D67" s="18">
         <v>45302</v>
       </c>
-      <c r="E67" s="22"/>
+      <c r="E67" s="3"/>
     </row>
     <row r="68" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
@@ -1993,14 +1986,14 @@
       <c r="D68" s="21">
         <v>45318</v>
       </c>
-      <c r="E68" s="22"/>
+      <c r="E68" s="3"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
-      <c r="E70" s="22"/>
+      <c r="E70" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -2009,76 +2002,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <cf401361b24e474cb011be6eb76c0e76 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Crown</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">69589897-2828-4761-976e-717fd8e631c9</TermId>
-        </TermInfo>
-      </Terms>
-    </cf401361b24e474cb011be6eb76c0e76>
-    <k85d23755b3a46b5a51451cf336b2e9b xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k85d23755b3a46b5a51451cf336b2e9b>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0dd52018-09d6-445c-a0bf-a7d393e3976c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Topic xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">Team Documents</Topic>
-    <HOMigrated xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">false</HOMigrated>
-    <ddeb1fd0a9ad4436a96525d34737dc44 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Defra Group</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0867f7b3-e76e-40ca-bb1f-5ba341a49230</TermId>
-        </TermInfo>
-      </Terms>
-    </ddeb1fd0a9ad4436a96525d34737dc44>
-    <lae2bfa7b6474897ab4a53f76ea236c7 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">14c80daa-741b-422c-9722-f71693c9ede4</TermId>
-        </TermInfo>
-      </Terms>
-    </lae2bfa7b6474897ab4a53f76ea236c7>
-    <TaxCatchAll xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Value>5</Value>
-      <Value>3</Value>
-      <Value>2</Value>
-      <Value>1</Value>
-      <Value>7</Value>
-    </TaxCatchAll>
-    <fe59e9859d6a491389c5b03567f5dda5 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">EA</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d5f78ddb-b1b6-4328-9877-d7e3ed06fdac</TermId>
-        </TermInfo>
-      </Terms>
-    </fe59e9859d6a491389c5b03567f5dda5>
-    <Team xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">West Midlands Flood Resilience</Team>
-    <n7493b4506bf40e28c373b1e51a33445 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Team</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">ff0485df-0575-416f-802f-e999165821b7</TermId>
-        </TermInfo>
-      </Terms>
-    </n7493b4506bf40e28c373b1e51a33445>
-    <SharedWithUsers xmlns="3706cc3d-17f7-47fa-8868-0fddc39686e3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false" LastSyncTimeStamp="2022-12-23T12:39:58.22Z"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Defra document" ma:contentTypeID="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC0100C9D7CF3DB3A5294495E668133806889C" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d902eb373446766bbf1ab3ec0f91b734">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="662745e8-e224-48e8-a2e3-254862b8c2f5" xmlns:ns3="0dd52018-09d6-445c-a0bf-a7d393e3976c" xmlns:ns4="3706cc3d-17f7-47fa-8868-0fddc39686e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7d15225178a027aa0bf830356bf0872" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="662745e8-e224-48e8-a2e3-254862b8c2f5"/>
@@ -2396,33 +2333,93 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false" LastSyncTimeStamp="2022-12-23T12:39:58.22Z"/>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <cf401361b24e474cb011be6eb76c0e76 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Crown</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">69589897-2828-4761-976e-717fd8e631c9</TermId>
+        </TermInfo>
+      </Terms>
+    </cf401361b24e474cb011be6eb76c0e76>
+    <k85d23755b3a46b5a51451cf336b2e9b xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k85d23755b3a46b5a51451cf336b2e9b>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0dd52018-09d6-445c-a0bf-a7d393e3976c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Topic xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">Team Documents</Topic>
+    <HOMigrated xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">false</HOMigrated>
+    <ddeb1fd0a9ad4436a96525d34737dc44 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Defra Group</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0867f7b3-e76e-40ca-bb1f-5ba341a49230</TermId>
+        </TermInfo>
+      </Terms>
+    </ddeb1fd0a9ad4436a96525d34737dc44>
+    <lae2bfa7b6474897ab4a53f76ea236c7 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">14c80daa-741b-422c-9722-f71693c9ede4</TermId>
+        </TermInfo>
+      </Terms>
+    </lae2bfa7b6474897ab4a53f76ea236c7>
+    <TaxCatchAll xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Value>5</Value>
+      <Value>3</Value>
+      <Value>2</Value>
+      <Value>1</Value>
+      <Value>7</Value>
+    </TaxCatchAll>
+    <fe59e9859d6a491389c5b03567f5dda5 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">EA</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d5f78ddb-b1b6-4328-9877-d7e3ed06fdac</TermId>
+        </TermInfo>
+      </Terms>
+    </fe59e9859d6a491389c5b03567f5dda5>
+    <Team xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">West Midlands Flood Resilience</Team>
+    <n7493b4506bf40e28c373b1e51a33445 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Team</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">ff0485df-0575-416f-802f-e999165821b7</TermId>
+        </TermInfo>
+      </Terms>
+    </n7493b4506bf40e28c373b1e51a33445>
+    <SharedWithUsers xmlns="3706cc3d-17f7-47fa-8868-0fddc39686e3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABFDC2C6-1282-4AD8-85C0-3BFC2D82127B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7CB7080-93A0-4465-A6CA-3DE4F8BEE390}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="662745e8-e224-48e8-a2e3-254862b8c2f5"/>
-    <ds:schemaRef ds:uri="0dd52018-09d6-445c-a0bf-a7d393e3976c"/>
-    <ds:schemaRef ds:uri="3706cc3d-17f7-47fa-8868-0fddc39686e3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F171807-FEE5-4AEA-A638-7AEBE7A4AFFE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65740454-FCBB-4306-863D-880BA6829E5F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2442,18 +2439,14 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F171807-FEE5-4AEA-A638-7AEBE7A4AFFE}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABFDC2C6-1282-4AD8-85C0-3BFC2D82127B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7CB7080-93A0-4465-A6CA-3DE4F8BEE390}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="662745e8-e224-48e8-a2e3-254862b8c2f5"/>
+    <ds:schemaRef ds:uri="0dd52018-09d6-445c-a0bf-a7d393e3976c"/>
+    <ds:schemaRef ds:uri="3706cc3d-17f7-47fa-8868-0fddc39686e3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>